<commit_message>
update json and pdf
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/OpenLisCS/21.01.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/OpenLisCS/21.01.00/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasalemm\Documents\GitHub\it-fse-accreditamento\GATEWAY\S1#111ENGINNERING\Engineering_Ingegneria_Informatica_S.p.A\OpenLisCS\21.01.00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1752D66A-535D-4378-841C-CE1143E24A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8525534B-9D8C-42BA-ACB4-63453671BCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-4965" windowWidth="29040" windowHeight="15840" xr2:uid="{0B6E9DF6-294C-4393-B56D-BCD2E58354B0}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -156,12 +156,6 @@
 </t>
   </si>
   <si>
-    <t>642fa1e33448bed3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.12b8b99d673bad876d8e828d6553965374269e34fe4fdfb96daf6da02e12b775.ff28be1416^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -177,12 +171,6 @@
 </t>
   </si>
   <si>
-    <t>6d336b6aabc2a6ff</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.9c7b3d1c734ab3a5bf39b9337f0c675765cf3df852c6fc4295db68ea61ab123e.408370f0f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
   </si>
   <si>
@@ -192,12 +180,6 @@
 </t>
   </si>
   <si>
-    <t>840f6571acc30a99</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.6f4e332ef40632392fef9c40adc3e759c829eea8a5e03fb962de593edcbd2af2.04677e9891^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
   </si>
   <si>
@@ -214,12 +196,6 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 5" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
-  </si>
-  <si>
-    <t>7841e6cb7dec3002</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.100da556c90d3e36c85bf377323639913171844643fb0a3279e304659f81a6f5.7947a40828^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -354,12 +330,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>bca85c260bef830f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.47b46284b3ad059500b8f6f13be9ce4762025403c4100b12a31226b4e822cd0f.d199f1d738^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT9_KO</t>
   </si>
   <si>
@@ -394,12 +364,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>faa70eb3b9b14162</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.a2d19267635106702a4198887335a8b066c20b349ee0bd0f9c1a74d72cb8818d.d39f87bda5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT13_KO</t>
   </si>
   <si>
@@ -407,12 +371,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>e1f73e13d0619922</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.a2d19267635106702a4198887335a8b066c20b349ee0bd0f9c1a74d72cb8818d.2e4f17e715^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT14_KO</t>
   </si>
   <si>
@@ -420,12 +378,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>33378ff22a5d0dc2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.a2d19267635106702a4198887335a8b066c20b349ee0bd0f9c1a74d72cb8818d.2dda72c5e4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LAB_CT15_KO</t>
   </si>
   <si>
@@ -440,13 +392,85 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>78a729c439f3bfce</t>
-  </si>
-  <si>
-    <t>feab517629483510</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e91e133d4ae03ea06dff65e5ce2cc352dbef4210a138bec4287bb6e242fa6595.461851fc65^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-01-18T17:10:18Z</t>
+  </si>
+  <si>
+    <t>2f5618d7cd71b168</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.ac5b7220c802388634c15c9df62c69ed92f43e9209581741da3db795fe85390e.9697eadfd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T12:17:59Z</t>
+  </si>
+  <si>
+    <t>9d954312fd41a79b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.fa6e59ddeb6183b35d1bac873f4a622a199a1c60093c90c2745e278b6f95a58e.97a31a3660^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T12:27:31Z</t>
+  </si>
+  <si>
+    <t>78151a0ba0a4005d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f30f6c3edfd95cebb73781dbfc48e6e6770d4f617471fc320dedc0c5d2cd00b6.72319e74b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T13:30:41Z</t>
+  </si>
+  <si>
+    <t>ac65c293ef8e3616</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.cea8d86d297d84eb74f80b70446d6d96142388b4823a4ceedaef639276342ae3.18204ee87c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T15:03:49Z</t>
+  </si>
+  <si>
+    <t>abc3a9c26ac809ee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.8dbde9d64d969b7f0b7300d5624cef0a26fa49ae0af5d6dd0041c31f40c1b97e.66bd320752^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T15:21:24Z</t>
+  </si>
+  <si>
+    <t>d7a9d434b5960a51</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>2023-02-03T16:01:04Z</t>
+  </si>
+  <si>
+    <t>In questo caso viene visualizzato l'errore 'Errore di validazione : Campo token JWT non valido' e il referto non viene prodotto</t>
+  </si>
+  <si>
+    <t>ea9aef3e2fcd4934</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f1b3f373486c71079664d118f6b4012164923450554622e9e3fed97602d67bab.da17c24ad9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T16:39:56Z</t>
+  </si>
+  <si>
+    <t>In questo caso viene visualizzato l'errore 'Errore di validazione : Errore semantico' e il referto non viene prodotto</t>
+  </si>
+  <si>
+    <t>355c7c82e6d6d351</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.f1b3f373486c71079664d118f6b4012164923450554622e9e3fed97602d67bab.1c197b8fee^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T17:00:18Z</t>
   </si>
 </sst>
 </file>
@@ -955,7 +979,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -965,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BF708B-A3B4-47EF-BF32-392DC634DEA8}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,6 +999,7 @@
     <col min="4" max="4" width="39.42578125" customWidth="1"/>
     <col min="5" max="5" width="52" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="75.140625" customWidth="1"/>
     <col min="10" max="10" width="42.85546875" customWidth="1"/>
@@ -1059,21 +1084,23 @@
         <v>18</v>
       </c>
       <c r="F3" s="13">
-        <v>44945</v>
-      </c>
-      <c r="G3" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="H3" s="14" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="16"/>
@@ -1090,27 +1117,29 @@
         <v>16</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="13">
-        <v>44945</v>
-      </c>
-      <c r="G4" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>70</v>
+      </c>
       <c r="H4" s="14" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="16"/>
@@ -1127,27 +1156,29 @@
         <v>16</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="13">
-        <v>44945</v>
-      </c>
-      <c r="G5" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="H5" s="14" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="16"/>
@@ -1164,27 +1195,29 @@
         <v>16</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F6" s="13">
-        <v>44952</v>
-      </c>
-      <c r="G6" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="H6" s="14" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M6" s="15"/>
       <c r="N6" s="16"/>
@@ -1201,27 +1234,29 @@
         <v>16</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F7" s="13">
-        <v>44945</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="H7" s="14" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="16"/>
@@ -1238,10 +1273,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="14"/>
@@ -1249,14 +1284,14 @@
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N8" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O8" s="17"/>
     </row>
@@ -1271,27 +1306,33 @@
         <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F9" s="13">
-        <v>44945</v>
-      </c>
-      <c r="G9" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="H9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
+      <c r="I9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="K9" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
       <c r="N9" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O9" s="17"/>
     </row>
@@ -1306,25 +1347,25 @@
         <v>16</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O10" s="17"/>
     </row>
@@ -1339,10 +1380,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
@@ -1350,14 +1391,14 @@
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L11" s="15"/>
       <c r="M11" s="15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O11" s="17"/>
     </row>
@@ -1372,27 +1413,33 @@
         <v>16</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F12" s="13">
         <v>44944</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="H12" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>83</v>
+      </c>
       <c r="K12" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
       <c r="N12" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O12" s="17"/>
     </row>
@@ -1407,29 +1454,25 @@
         <v>16</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="13">
-        <v>44944</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F13" s="13"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
+      <c r="M13" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="N13" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O13" s="17"/>
     </row>
@@ -1444,10 +1487,10 @@
         <v>16</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="14"/>
@@ -1455,14 +1498,14 @@
       <c r="I14" s="14"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O14" s="17"/>
     </row>
@@ -1477,10 +1520,10 @@
         <v>16</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="14"/>
@@ -1488,14 +1531,14 @@
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O15" s="17"/>
     </row>
@@ -1510,10 +1553,10 @@
         <v>16</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14"/>
@@ -1521,14 +1564,14 @@
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="N16" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O16" s="17"/>
     </row>
@@ -1543,29 +1586,25 @@
         <v>16</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="13">
-        <v>44944</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F17" s="13"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
+      <c r="M17" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="N17" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O17" s="17"/>
     </row>
@@ -1580,29 +1619,33 @@
         <v>16</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F18" s="13">
-        <v>44944</v>
-      </c>
-      <c r="G18" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="H18" s="14" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="J18" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="K18" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O18" s="17"/>
     </row>
@@ -1617,29 +1660,33 @@
         <v>16</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="F19" s="13">
-        <v>44944</v>
-      </c>
-      <c r="G19" s="14"/>
+        <v>44960</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>90</v>
+      </c>
       <c r="H19" s="14" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="J19" s="15"/>
+        <v>89</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="K19" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
       <c r="N19" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O19" s="17"/>
     </row>
@@ -1654,10 +1701,10 @@
         <v>16</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="14"/>
@@ -1665,14 +1712,14 @@
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L20" s="15"/>
       <c r="M20" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O20" s="17"/>
     </row>
@@ -1687,10 +1734,10 @@
         <v>16</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14"/>
@@ -1698,14 +1745,14 @@
       <c r="I21" s="14"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="N21" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O21" s="17"/>
     </row>

</xml_diff>